<commit_message>
added 2nd join to camrule but need to update logic to pull pricing
</commit_message>
<xml_diff>
--- a/rx_PSC_TenantPricing.xlsx
+++ b/rx_PSC_TenantPricing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-TenantPricingYSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E19EFE-C29C-460C-A3DC-A3E9E63CFCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F79167E-DA76-4BF2-BAD8-D8783B269B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14250" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>&amp;=display.UnitRent</t>
   </si>
   <si>
-    <t>&amp;=display.TotalUnits</t>
-  </si>
-  <si>
     <t>&amp;=display.StartOcc</t>
   </si>
   <si>
@@ -59,12 +56,6 @@
     <t>&amp;=display.NetOcc</t>
   </si>
   <si>
-    <t>&amp;=display.EndOcc</t>
-  </si>
-  <si>
-    <t>&amp;=display.FutureRes</t>
-  </si>
-  <si>
     <t>&amp;=header.PropertyName</t>
   </si>
   <si>
@@ -92,9 +83,6 @@
     <t>&amp;=&amp;=SUM(J5:J{-1})</t>
   </si>
   <si>
-    <t>&amp;=&amp;=IF(A5=A{-1}, 0,1)</t>
-  </si>
-  <si>
     <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, D5:D{-1})</t>
   </si>
   <si>
@@ -129,6 +117,18 @@
   </si>
   <si>
     <t>Tenant Pricing Report</t>
+  </si>
+  <si>
+    <t>&amp;=display.resident</t>
+  </si>
+  <si>
+    <t>&amp;=display.status</t>
+  </si>
+  <si>
+    <t>&amp;=display.MoveIn</t>
+  </si>
+  <si>
+    <t>&amp;=display.MoveOut</t>
   </si>
 </sst>
 </file>
@@ -232,11 +232,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +557,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -566,149 +566,149 @@
     <col min="2" max="2" width="17.90625" customWidth="1"/>
     <col min="3" max="3" width="7.7265625" customWidth="1"/>
     <col min="4" max="4" width="28.6328125" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
     <col min="6" max="6" width="8.453125" customWidth="1"/>
     <col min="7" max="7" width="9.7265625" customWidth="1"/>
     <col min="8" max="8" width="7.54296875" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" customWidth="1"/>
+    <col min="9" max="9" width="11.08984375" customWidth="1"/>
     <col min="10" max="10" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added header and modified excel template
</commit_message>
<xml_diff>
--- a/rx_PSC_TenantPricing.xlsx
+++ b/rx_PSC_TenantPricing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-TenantPricingYSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4612B7D-0407-47AF-8849-EE216CEC6F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBA5ECC-8516-4852-A626-021E7415E476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14250" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>&amp;=display.UnitType</t>
   </si>
@@ -44,15 +44,6 @@
     <t>&amp;=display.UnitRent</t>
   </si>
   <si>
-    <t>&amp;=display.StartOcc</t>
-  </si>
-  <si>
-    <t>&amp;=display.MoveOuts</t>
-  </si>
-  <si>
-    <t>&amp;=display.NetOcc</t>
-  </si>
-  <si>
     <t>&amp;=header.PropertyName</t>
   </si>
   <si>
@@ -65,9 +56,6 @@
     <t>&amp;=&amp;=SUM(G5:G{-1})</t>
   </si>
   <si>
-    <t>&amp;=&amp;=SUM(H5:H{-1})</t>
-  </si>
-  <si>
     <t>Tenant</t>
   </si>
   <si>
@@ -117,6 +105,15 @@
   </si>
   <si>
     <t>&amp;=display.CurrentPrice</t>
+  </si>
+  <si>
+    <t>&amp;=display.LastPriceChangeDate</t>
+  </si>
+  <si>
+    <t>&amp;=display.LastPrice</t>
+  </si>
+  <si>
+    <t>&amp;=display.Discount_Desc</t>
   </si>
 </sst>
 </file>
@@ -171,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -188,27 +185,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,155 +522,155 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" customWidth="1"/>
-    <col min="4" max="4" width="28.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="6" width="17.90625" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" customWidth="1"/>
-    <col min="8" max="8" width="7.54296875" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" customWidth="1"/>
+    <col min="8" max="8" width="24.6328125" customWidth="1"/>
+    <col min="9" max="9" width="14.6328125" customWidth="1"/>
     <col min="10" max="10" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="H4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="I4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="J4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="G5" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E11" s="5"/>
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="990" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>

</xml_diff>

<commit_message>
yaaaaaaa (runs to screen)
</commit_message>
<xml_diff>
--- a/rx_PSC_TenantPricing.xlsx
+++ b/rx_PSC_TenantPricing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-TenantPricingYSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBA5ECC-8516-4852-A626-021E7415E476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2BCD25-42FC-4CAE-A780-8D281FD4DD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14250" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -189,19 +189,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,7 +523,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -540,76 +541,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -638,10 +639,10 @@
       <c r="H5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="6" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating dates  - needs work still
</commit_message>
<xml_diff>
--- a/rx_PSC_TenantPricing.xlsx
+++ b/rx_PSC_TenantPricing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-TenantPricingYSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14A5E5D-2CAA-4CE0-8A27-90F434ED2C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF447F7-B90B-45E1-9246-E39718FBF5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14250" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <t>&amp;=display.LastPrice</t>
   </si>
   <si>
-    <t>&amp;=display.Discount_Desc</t>
+    <t>&amp;=display.Promotions</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
need to update v2 to only show discounts applied to the tenant
</commit_message>
<xml_diff>
--- a/rx_PSC_TenantPricing.xlsx
+++ b/rx_PSC_TenantPricing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-TenantPricingYSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF447F7-B90B-45E1-9246-E39718FBF5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0833B44-2049-4CF2-B183-D932280AAB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14250" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <t>&amp;=display.LastPrice</t>
   </si>
   <si>
-    <t>&amp;=display.Promotions</t>
+    <t>&amp;=display.Discount_Desc</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added unit type price column and logic to display current price as last price if last updated price has no changes
</commit_message>
<xml_diff>
--- a/rx_PSC_TenantPricing.xlsx
+++ b/rx_PSC_TenantPricing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-TenantPricingYSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0833B44-2049-4CF2-B183-D932280AAB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F25038-0EDA-4281-B7B0-B60800B477E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>&amp;=display.UnitType</t>
   </si>
@@ -114,12 +114,27 @@
   </si>
   <si>
     <t>&amp;=display.Discount_Desc</t>
+  </si>
+  <si>
+    <t>Unit Type</t>
+  </si>
+  <si>
+    <t>&amp;=display.UTPrice</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>&amp;=display.uscode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -189,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -203,6 +218,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,27 +536,29 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7265625" customWidth="1"/>
     <col min="2" max="2" width="11.90625" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" customWidth="1"/>
-    <col min="6" max="6" width="11.1796875" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" customWidth="1"/>
-    <col min="8" max="8" width="24.6328125" customWidth="1"/>
-    <col min="9" max="9" width="14.6328125" customWidth="1"/>
-    <col min="10" max="10" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" customWidth="1"/>
+    <col min="10" max="10" width="24.6328125" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -553,8 +571,10 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -567,8 +587,10 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -581,8 +603,10 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -590,31 +614,37 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -622,31 +652,37 @@
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -655,22 +691,24 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="990" orientation="portrait" useFirstPageNumber="1"/>
@@ -682,7 +720,7 @@
     <brk id="29" max="16383" man="1"/>
   </rowBreaks>
   <ignoredErrors>
-    <ignoredError sqref="C6" numberStoredAsText="1"/>
+    <ignoredError sqref="D6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>